<commit_message>
Comecei a fechar o delay do reconhecimento. Falta apenas incluir o nome da pessoa pra que funcione bem com 2 ou mais sendo reconhecidos.
</commit_message>
<xml_diff>
--- a/Validacao_de_Pessoas/Presenca.xlsx
+++ b/Validacao_de_Pessoas/Presenca.xlsx
@@ -348,7 +348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -417,6 +417,28 @@
         </is>
       </c>
       <c r="D3" t="inlineStr">
+        <is>
+          <t>ICA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Gabriel Taranto</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>ICA</t>
         </is>

</xml_diff>